<commit_message>
update app e dati
</commit_message>
<xml_diff>
--- a/lista_partiti_filled.xlsx
+++ b/lista_partiti_filled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_vari_miei\dati_simulatore_elettorale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED73470-52CA-4392-A54E-2B1EC93F9989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36478807-85C1-4B3F-84E4-22CCAAD2107F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>FDI</t>
   </si>
   <si>
-    <t>AZN</t>
-  </si>
-  <si>
     <t>ALTRI</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>SI-VERDI</t>
+  </si>
+  <si>
+    <t>AZIONE-IV</t>
   </si>
 </sst>
 </file>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>771490</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -628,7 +628,7 @@
         <v>654490</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
         <v>542238</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -658,7 +658,7 @@
         <v>404748</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -673,7 +673,7 @@
         <v>337562</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -688,7 +688,7 @@
         <v>318573</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
         <v>261931</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -718,7 +718,7 @@
         <v>199178</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,7 +733,7 @@
         <v>82982</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -748,7 +748,7 @@
         <v>57296</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -763,7 +763,7 @@
         <v>43965</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>37407</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -793,7 +793,7 @@
         <v>34747</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -808,7 +808,7 @@
         <v>33225</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,7 +823,7 @@
         <v>18411</v>
       </c>
       <c r="D16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -838,7 +838,7 @@
         <v>10133</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
         <v>5830</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -868,7 +868,7 @@
         <v>5232</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -883,7 +883,7 @@
         <v>4534</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -898,7 +898,7 @@
         <v>3376</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>2582</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -928,7 +928,7 @@
         <v>1270</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>1187</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -958,7 +958,7 @@
         <v>502</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -973,7 +973,7 @@
         <v>1489744</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1049,7 +1049,7 @@
         <v>1954821</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1109,7 +1109,7 @@
         <v>21777</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,7 +1124,7 @@
         <v>249364</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>